<commit_message>
Add test cases of special characters in language and skill name
</commit_message>
<xml_diff>
--- a/Test Cases - User Story 1 - Sprint 1.xlsx
+++ b/Test Cases - User Story 1 - Sprint 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Documents\IndustryConnect\InternShip\Mars\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Documents\IndustryConnect\GitRepository\test\Project.Mars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4512D436-F43D-486C-851F-18D1F6872FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68017B5-3899-47F3-B493-1196B8B10827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="297">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -1262,12 +1262,6 @@
   </si>
   <si>
     <t>1. Click the "Add New" button.
-2. Enter 2,000 characters in the "Add Skill" field.
-3. Choose a valid level in the "Choose Skill Level" selection box.
-4. Click the "Add" button.</t>
-  </si>
-  <si>
-    <t>1. Click the "Add New" button.
 2. Enter a script (e.g., "&lt;script&gt;alert('test');&lt;/script&gt;") in the "Add Skill" field.
 3. Choose a valid level in the "Choose Skill Level" selection box.
 4. Click the "Add" button.</t>
@@ -1373,10 +1367,6 @@
   </si>
   <si>
     <t>Choose Skill Level: "Beginner"</t>
-  </si>
-  <si>
-    <t>Add Skill: 2,000 characters
-Choose Skill Level: "Beginner"</t>
   </si>
   <si>
     <t>Add Skill: "&lt;script&gt;alert('test');&lt;/script&gt;"
@@ -1493,6 +1483,63 @@
   <si>
     <t>Email address: "jay.pounggmail.com"
 Password: "passwd123"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add language in name with special characters</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Click the "Add New" button.
+2. Enter special characters in the "Add Language" field.
+3. Choose a valid level in the "Choose Language Level" selection box.
+4. Click the "Add" button.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Language should not be added successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add Language: "/.,&amp;*$#@"
+Choose Language Level: "Basic"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_022</t>
+  </si>
+  <si>
+    <t>Add skill in name with special characters</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The user is on the Profile page.
+2. Skills section has been selected.
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Click the "Add New" button.
+2. Enter 2,000 characters in the "Add Skill" field.
+3. Choose a valid level in the "Choose Skill Level" selection box.
+4. Click the "Add" button.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Click the "Add New" button.
+2. Enter special characters in the "Add Skill" field.
+3. Choose a valid level in the "Choose Skill Level" selection box.
+4. Click the "Add" button.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add Skill: 2,000 characters
+Choose Skill Level: "Beginner"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add Skill: "/.,&amp;*$#@"
+Choose Skill Level: "Beginner"</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1644,6 +1691,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1661,16 +1718,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2031,28 +2078,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -2082,7 +2129,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>12</v>
@@ -2091,10 +2138,10 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="138" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -2119,8 +2166,8 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="138" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="13"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
@@ -2143,8 +2190,8 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="138" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="7" t="s">
         <v>31</v>
       </c>
@@ -2167,8 +2214,8 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="138" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="13"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
@@ -2191,8 +2238,8 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="138" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="13"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
@@ -2215,8 +2262,8 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="165.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="7" t="s">
         <v>34</v>
       </c>
@@ -2239,8 +2286,8 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="151.80000000000001" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="7" t="s">
         <v>35</v>
       </c>
@@ -2263,8 +2310,8 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="13"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="7" t="s">
         <v>36</v>
       </c>
@@ -2330,7 +2377,7 @@
         <v>54</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>55</v>
@@ -2633,28 +2680,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -2665,10 +2712,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>109</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2684,7 +2731,7 @@
         <v>69</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>70</v>
@@ -2693,8 +2740,8 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
@@ -2708,7 +2755,7 @@
         <v>107</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>108</v>
@@ -2717,10 +2764,10 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="16" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -2736,7 +2783,7 @@
         <v>72</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>73</v>
@@ -2745,13 +2792,13 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>67</v>
@@ -2760,7 +2807,7 @@
         <v>74</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>75</v>
@@ -2769,22 +2816,22 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="13"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>67</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>75</v>
@@ -2793,8 +2840,8 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="13"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
@@ -2808,7 +2855,7 @@
         <v>77</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>78</v>
@@ -2817,8 +2864,8 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="3" t="s">
         <v>34</v>
       </c>
@@ -2841,8 +2888,8 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
@@ -2856,7 +2903,7 @@
         <v>83</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>58</v>
@@ -2865,8 +2912,8 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="13"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="3" t="s">
         <v>36</v>
       </c>
@@ -2880,7 +2927,7 @@
         <v>85</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>87</v>
@@ -2889,8 +2936,8 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="13"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
@@ -2913,8 +2960,8 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="13"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="3" t="s">
         <v>56</v>
       </c>
@@ -2937,8 +2984,8 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="13"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="3" t="s">
         <v>106</v>
       </c>
@@ -3263,11 +3310,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB331B0D-6616-41F2-88C6-0DEB00AF68FB}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3275,7 +3322,7 @@
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="74.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
-    <col min="4" max="4" width="75.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.44140625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49.21875" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
@@ -3285,28 +3332,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -3317,10 +3364,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>191</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -3345,8 +3392,8 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
@@ -3369,10 +3416,10 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="16" t="s">
         <v>192</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -3397,8 +3444,8 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
@@ -3421,8 +3468,8 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="13"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="3" t="s">
         <v>32</v>
       </c>
@@ -3435,7 +3482,7 @@
       <c r="F6" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>123</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -3445,46 +3492,858 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="13"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>258</v>
+        <v>286</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>111</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>126</v>
+        <v>287</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>127</v>
+        <v>289</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>64</v>
+        <v>288</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="13"/>
+    <row r="8" spans="1:10" ht="69" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>128</v>
+        <v>257</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>111</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>129</v>
       </c>
+      <c r="G9" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="69" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" ht="137.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="69" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="69" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="A4:A10"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I38" xr:uid="{0D3F7C49-AECD-4BCF-AD14-2981E8382D9B}">
+      <formula1>"In-Progress,UnExecuted,Block"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J38" xr:uid="{65F8B735-7E81-4F76-A4FC-4D9F7BB54F05}">
+      <formula1>"Pass,Fail"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8568EF4B-A638-4EBA-90D3-9792D794FF43}">
+  <dimension ref="A1:J36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="75.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.21875" customWidth="1"/>
+    <col min="7" max="7" width="39" customWidth="1"/>
+    <col min="8" max="8" width="55.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="69" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="69" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="69" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="69" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>238</v>
+      </c>
       <c r="G8" s="4" t="s">
-        <v>130</v>
+        <v>259</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>131</v>
@@ -3493,22 +4352,22 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="14"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>137</v>
+      <c r="D9" s="11" t="s">
+        <v>213</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>111</v>
+        <v>255</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>132</v>
+        <v>239</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>133</v>
+        <v>260</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>134</v>
@@ -3516,201 +4375,201 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="69" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>135</v>
+        <v>215</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>111</v>
+        <v>255</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>136</v>
+        <v>240</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>112</v>
+        <v>264</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>190</v>
+      <c r="B11" s="16" t="s">
+        <v>216</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>138</v>
+        <v>217</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>152</v>
+        <v>241</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>160</v>
+        <v>270</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>159</v>
+        <v>218</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="13"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>139</v>
+        <v>219</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>152</v>
+        <v>241</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>159</v>
+        <v>218</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="14"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="3" t="s">
         <v>106</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>140</v>
+        <v>220</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>152</v>
+        <v>241</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>179</v>
+        <v>244</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>161</v>
+        <v>245</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>159</v>
+        <v>218</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>187</v>
+      <c r="B14" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>146</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>167</v>
+        <v>222</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>164</v>
+        <v>246</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>178</v>
+        <v>247</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>168</v>
+        <v>248</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>158</v>
+        <v>209</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="13"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="3" t="s">
         <v>147</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>166</v>
+        <v>223</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>164</v>
+        <v>246</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>177</v>
+        <v>249</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>169</v>
+        <v>250</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>158</v>
+        <v>209</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="137.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="13"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="3" t="s">
         <v>148</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>141</v>
+        <v>224</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>152</v>
+        <v>241</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>163</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4" t="s">
-        <v>165</v>
+        <v>225</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="13"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="3" t="s">
         <v>149</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>142</v>
+        <v>226</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>152</v>
+        <v>241</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>171</v>
+        <v>251</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>173</v>
+        <v>261</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>131</v>
@@ -3719,22 +4578,22 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="13"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="3" t="s">
         <v>150</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>143</v>
+        <v>227</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>152</v>
+        <v>241</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>174</v>
+        <v>252</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>172</v>
+        <v>262</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>134</v>
@@ -3743,22 +4602,22 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="3" t="s">
         <v>151</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>144</v>
+        <v>228</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>152</v>
+        <v>241</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>175</v>
+        <v>253</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>176</v>
+        <v>263</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>64</v>
@@ -3766,79 +4625,69 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="69" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>195</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>188</v>
+        <v>229</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>153</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>145</v>
+        <v>230</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>152</v>
+        <v>274</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>181</v>
+        <v>254</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>112</v>
+        <v>264</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>182</v>
+        <v>231</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>186</v>
+      <c r="B21" s="9" t="s">
+        <v>232</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>155</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>199</v>
+        <v>273</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>197</v>
+        <v>274</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>201</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>202</v>
+        <v>233</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>201</v>
-      </c>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="4" t="s">
-        <v>203</v>
-      </c>
+      <c r="H22" s="3"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
@@ -3855,9 +4704,9 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
       <c r="D24" s="7"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -3867,9 +4716,9 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="7"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -3927,9 +4776,9 @@
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
       <c r="D30" s="7"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -3939,9 +4788,9 @@
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="7"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -4010,775 +4859,21 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
+  <mergeCells count="6">
+    <mergeCell ref="A14:A19"/>
     <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="A11:A13"/>
     <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A4:A9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I37" xr:uid="{0D3F7C49-AECD-4BCF-AD14-2981E8382D9B}">
-      <formula1>"In-Progress,UnExecuted,Block"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J37" xr:uid="{65F8B735-7E81-4F76-A4FC-4D9F7BB54F05}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J36" xr:uid="{C9ED0A77-F2FF-4FD5-9F04-9F299BF1BED7}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8568EF4B-A638-4EBA-90D3-9792D794FF43}">
-  <dimension ref="A1:J35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" customWidth="1"/>
-    <col min="4" max="4" width="75.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.21875" customWidth="1"/>
-    <col min="7" max="7" width="39" customWidth="1"/>
-    <col min="8" max="8" width="55.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" ht="137.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" ht="69" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J35" xr:uid="{C9ED0A77-F2FF-4FD5-9F04-9F299BF1BED7}">
-      <formula1>"Pass,Fail"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I35" xr:uid="{345A0392-218A-46B0-B290-F5A362E22842}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I36" xr:uid="{345A0392-218A-46B0-B290-F5A362E22842}">
       <formula1>"In-Progress,UnExecuted,Block"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>